<commit_message>
update ppt + word
</commit_message>
<xml_diff>
--- a/Nhóm-10-Bảng-kế-hoạch.xlsx
+++ b/Nhóm-10-Bảng-kế-hoạch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project Gia Pha\Tao-Cay-Gia-Pha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studying\CTDL-GT\Lưu Trữ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52934AB0-73FE-4CF2-87FE-F0D428C844FF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CE4B4A-72FD-401C-B993-B5F50A64EC84}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kế Hoạch" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="151">
   <si>
     <t>DOB</t>
   </si>
@@ -1416,6 +1416,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1424,33 +1451,6 @@
     </xf>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1458,6 +1458,700 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="38">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right/>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right/>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="7" tint="-0.499984740745262"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right/>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top style="thick">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="0"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1799,25 +2493,25 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thick">
-          <color rgb="FF0070C0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="dashed">
+          <color auto="1"/>
+        </right>
+        <top style="thick">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="dashed">
-          <color auto="1"/>
-        </right>
-        <top style="thick">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
+      <border>
+        <bottom style="thick">
+          <color rgb="FF0070C0"/>
         </bottom>
       </border>
     </dxf>
@@ -1853,700 +2547,6 @@
         <horizontal/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right/>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right/>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="7" tint="-0.499984740745262"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right/>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top style="thick">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="0"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2561,49 +2561,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:K25" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:K25" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35">
   <autoFilter ref="A2:K25" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="STT" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="DANH SÁCH CÔNG VIỆC" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="NỘI DUNG CHI TIẾT CÔNG VIỆC" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Nguyễn Lê Nguyên Anh" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{0921F172-22AF-4D48-BB40-4D1750CEFAA0}" name="Trần Gia Hân" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Võ Thành Văn" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="GHI CHÚ" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Ngày bắt đầu (dự kiến)" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Ngày kết thúc (dự kiến)" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Ngày bắt đầu (thực tế)" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Ngày kết thúc (thực tế)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="STT" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="DANH SÁCH CÔNG VIỆC" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="NỘI DUNG CHI TIẾT CÔNG VIỆC" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Nguyễn Lê Nguyên Anh" dataDxfId="31"/>
+    <tableColumn id="12" xr3:uid="{0921F172-22AF-4D48-BB40-4D1750CEFAA0}" name="Trần Gia Hân" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Võ Thành Văn" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="GHI CHÚ" dataDxfId="28"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Ngày bắt đầu (dự kiến)" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Ngày kết thúc (dự kiến)" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Ngày bắt đầu (thực tế)" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Ngày kết thúc (thực tế)" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:T1048560" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:T1048560" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20">
   <autoFilter ref="A1:T1048560" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="THE HE" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="HO VA TEN" dataDxfId="32"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="CHUC VU" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="DOB" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="NAM MAT" dataDxfId="29"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="GIOI TINH" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="TEN CHA" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="TEN ME" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="TT TRONG GD" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="TEN ANH" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="TEN CHI" dataDxfId="23"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="TEN EM TRAI" dataDxfId="22"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="TEN EM GAI" dataDxfId="21"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="HON NHAN" dataDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="TEN VO - CHONG" dataDxfId="19"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="SO CON" dataDxfId="18"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="CON TRAI" dataDxfId="17"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="CON GAI" dataDxfId="16"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="CONG TRANG" dataDxfId="15"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="PHAN MO" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="THE HE" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="HO VA TEN" dataDxfId="18"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="CHUC VU" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="DOB" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="NAM MAT" dataDxfId="15"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="GIOI TINH" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="TEN CHA" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="TEN ME" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="TT TRONG GD" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="TEN ANH" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="TEN CHI" dataDxfId="9"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="TEN EM TRAI" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="TEN EM GAI" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="HON NHAN" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="TEN VO - CHONG" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="SO CON" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="CON TRAI" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="CON GAI" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="CONG TRANG" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="PHAN MO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2874,41 +2874,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" style="23" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="45.5703125" style="24" customWidth="1"/>
-    <col min="4" max="5" width="25.7109375" style="55" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="25" customWidth="1"/>
-    <col min="7" max="7" width="33.28515625" style="25" hidden="1" customWidth="1"/>
-    <col min="8" max="11" width="14.7109375" style="89" customWidth="1"/>
-    <col min="12" max="22" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.5546875" style="24" customWidth="1"/>
+    <col min="4" max="5" width="25.6640625" style="55" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="33.33203125" style="25" hidden="1" customWidth="1"/>
+    <col min="8" max="11" width="14.6640625" style="89" customWidth="1"/>
+    <col min="12" max="22" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="21" customFormat="1" ht="34.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="93" t="s">
+    <row r="1" spans="1:22" s="21" customFormat="1" ht="34.200000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="95"/>
-    </row>
-    <row r="2" spans="1:22" s="21" customFormat="1" ht="43.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="104"/>
+    </row>
+    <row r="2" spans="1:22" s="21" customFormat="1" ht="43.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="77" t="s">
         <v>4</v>
       </c>
@@ -2944,7 +2944,7 @@
       </c>
       <c r="L2" s="91"/>
     </row>
-    <row r="3" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="78">
         <v>1</v>
       </c>
@@ -2984,7 +2984,7 @@
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" s="2" customFormat="1" ht="19.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" s="2" customFormat="1" ht="19.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="79">
         <v>2</v>
       </c>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="L4" s="92"/>
     </row>
-    <row r="5" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="80">
         <v>3</v>
       </c>
@@ -3048,7 +3048,7 @@
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
     </row>
-    <row r="6" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="80">
         <v>4</v>
       </c>
@@ -3084,7 +3084,7 @@
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
     </row>
-    <row r="7" spans="1:22" s="2" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" s="2" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="79">
         <v>5</v>
       </c>
@@ -3108,7 +3108,7 @@
       <c r="K7" s="88"/>
       <c r="L7" s="92"/>
     </row>
-    <row r="8" spans="1:22" s="2" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" s="2" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="79">
         <v>6</v>
       </c>
@@ -3134,7 +3134,7 @@
       <c r="K8" s="88"/>
       <c r="L8" s="92"/>
     </row>
-    <row r="9" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="80">
         <v>7</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>43404</v>
       </c>
       <c r="I9" s="87">
-        <v>43376</v>
+        <v>43407</v>
       </c>
       <c r="J9" s="87"/>
       <c r="K9" s="88"/>
@@ -3170,7 +3170,7 @@
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
     </row>
-    <row r="10" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="80">
         <v>8</v>
       </c>
@@ -3204,7 +3204,7 @@
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
     </row>
-    <row r="11" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="80">
         <v>9</v>
       </c>
@@ -3214,13 +3214,11 @@
       <c r="C11" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="58" t="s">
+      <c r="D11" s="58"/>
+      <c r="E11" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="58"/>
-      <c r="F11" s="60" t="s">
-        <v>119</v>
-      </c>
+      <c r="F11" s="60"/>
       <c r="G11" s="60"/>
       <c r="H11" s="87">
         <v>43372</v>
@@ -3244,7 +3242,7 @@
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
     </row>
-    <row r="12" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="80">
         <v>10</v>
       </c>
@@ -3280,7 +3278,7 @@
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
     </row>
-    <row r="13" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="80">
         <v>11</v>
       </c>
@@ -3318,7 +3316,7 @@
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
     </row>
-    <row r="14" spans="1:22" s="2" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" s="2" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="79">
         <v>12</v>
       </c>
@@ -3344,34 +3342,34 @@
       <c r="K14" s="88"/>
       <c r="L14" s="92"/>
     </row>
-    <row r="15" spans="1:22" s="2" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="96">
+    <row r="15" spans="1:22" s="2" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="93">
         <v>13</v>
       </c>
-      <c r="B15" s="97"/>
-      <c r="C15" s="98" t="s">
+      <c r="B15" s="94"/>
+      <c r="C15" s="95" t="s">
         <v>137</v>
       </c>
-      <c r="D15" s="99"/>
-      <c r="E15" s="100" t="s">
+      <c r="D15" s="96"/>
+      <c r="E15" s="97" t="s">
         <v>119</v>
       </c>
-      <c r="F15" s="101"/>
-      <c r="G15" s="102"/>
-      <c r="H15" s="103">
+      <c r="F15" s="98"/>
+      <c r="G15" s="99"/>
+      <c r="H15" s="100">
         <v>43386</v>
       </c>
-      <c r="I15" s="103">
+      <c r="I15" s="100">
         <v>43391</v>
       </c>
-      <c r="J15" s="103"/>
-      <c r="K15" s="104"/>
+      <c r="J15" s="100"/>
+      <c r="K15" s="101"/>
       <c r="L15" s="92"/>
       <c r="M15" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="80">
         <v>14</v>
       </c>
@@ -3409,7 +3407,7 @@
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
     </row>
-    <row r="17" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="80">
         <v>15</v>
       </c>
@@ -3445,7 +3443,7 @@
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
     </row>
-    <row r="18" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="80">
         <v>16</v>
       </c>
@@ -3483,7 +3481,7 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
     </row>
-    <row r="19" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="80">
         <v>17</v>
       </c>
@@ -3519,7 +3517,7 @@
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
     </row>
-    <row r="20" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="90">
         <v>18</v>
       </c>
@@ -3553,7 +3551,7 @@
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
     </row>
-    <row r="21" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="80">
         <v>19</v>
       </c>
@@ -3589,7 +3587,7 @@
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
     </row>
-    <row r="22" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="80">
         <v>20</v>
       </c>
@@ -3631,7 +3629,7 @@
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
     </row>
-    <row r="23" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="81">
         <v>21</v>
       </c>
@@ -3671,7 +3669,7 @@
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
     </row>
-    <row r="24" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="81">
         <v>22</v>
       </c>
@@ -3683,9 +3681,7 @@
       <c r="E24" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="F24" s="73" t="s">
-        <v>119</v>
-      </c>
+      <c r="F24" s="73"/>
       <c r="G24" s="60"/>
       <c r="H24" s="87">
         <v>43407</v>
@@ -3707,7 +3703,7 @@
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
     </row>
-    <row r="25" spans="1:22" s="22" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" s="22" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="80" t="s">
         <v>7</v>
       </c>
@@ -3756,26 +3752,26 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" style="8" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="28" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="5" customWidth="1"/>
-    <col min="4" max="5" width="12.7109375" style="10" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="10" customWidth="1"/>
-    <col min="7" max="8" width="20.7109375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="10" customWidth="1"/>
-    <col min="10" max="13" width="20.7109375" style="5" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" style="10" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" style="32" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" style="10" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" style="36" customWidth="1"/>
-    <col min="18" max="18" width="20.7109375" style="44" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" style="5" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" style="5" customWidth="1"/>
+    <col min="4" max="5" width="12.6640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="10" customWidth="1"/>
+    <col min="7" max="8" width="20.6640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="10" customWidth="1"/>
+    <col min="10" max="13" width="20.6640625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" style="10" customWidth="1"/>
+    <col min="15" max="15" width="20.6640625" style="32" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" style="10" customWidth="1"/>
+    <col min="17" max="17" width="20.6640625" style="36" customWidth="1"/>
+    <col min="18" max="18" width="20.6640625" style="44" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" style="5" customWidth="1"/>
+    <col min="20" max="20" width="20.6640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="40" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="40" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="38" t="s">
         <v>8</v>
       </c>
@@ -3837,7 +3833,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -3885,7 +3881,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="49"/>
       <c r="C3" s="45"/>
       <c r="N3" s="19"/>
@@ -3896,7 +3892,7 @@
       <c r="R3" s="50"/>
       <c r="S3" s="45"/>
     </row>
-    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>51</v>
       </c>
@@ -3928,7 +3924,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15"/>
       <c r="B5" s="26"/>
       <c r="C5" s="16"/>
@@ -3952,7 +3948,7 @@
       <c r="S5" s="16"/>
       <c r="T5" s="18"/>
     </row>
-    <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>2</v>
       </c>
@@ -4004,7 +4000,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="48" t="s">
         <v>30</v>
       </c>
@@ -4048,14 +4044,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="45"/>
       <c r="N8" s="19"/>
       <c r="Q8" s="36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="27" t="s">
         <v>52</v>
@@ -4101,7 +4097,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="28" t="s">
         <v>53</v>
       </c>
@@ -4139,7 +4135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="15"/>
       <c r="B11" s="26"/>
       <c r="C11" s="16"/>
@@ -4163,7 +4159,7 @@
       <c r="S11" s="16"/>
       <c r="T11" s="18"/>
     </row>
-    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>3</v>
       </c>
@@ -4215,7 +4211,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="28" t="s">
         <v>32</v>
       </c>
@@ -4253,7 +4249,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="48" t="s">
         <v>33</v>
       </c>
@@ -4291,7 +4287,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="28" t="s">
         <v>36</v>
       </c>
@@ -4329,7 +4325,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="48" t="s">
         <v>34</v>
       </c>
@@ -4364,7 +4360,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="28" t="s">
         <v>54</v>
       </c>
@@ -4408,7 +4404,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="28" t="s">
         <v>47</v>
       </c>
@@ -4440,7 +4436,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="49"/>
       <c r="B19" s="28" t="s">
         <v>49</v>
@@ -4480,7 +4476,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="51"/>
       <c r="B20" s="26" t="s">
         <v>55</v>
@@ -4524,7 +4520,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
         <v>4</v>
       </c>
@@ -4570,7 +4566,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B22" s="48" t="s">
         <v>37</v>
       </c>
@@ -4614,7 +4610,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B23" s="28" t="s">
         <v>38</v>
       </c>
@@ -4644,7 +4640,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B24" s="48" t="s">
         <v>39</v>
       </c>
@@ -4680,7 +4676,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B25" s="28" t="s">
         <v>40</v>
       </c>
@@ -4710,7 +4706,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B26" s="48" t="s">
         <v>41</v>
       </c>
@@ -4754,7 +4750,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
       <c r="B27" s="27" t="s">
         <v>95</v>
@@ -4798,7 +4794,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="28" t="s">
         <v>96</v>
       </c>
@@ -4836,7 +4832,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="28" t="s">
         <v>97</v>
       </c>
@@ -4868,7 +4864,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="15"/>
       <c r="B30" s="26" t="s">
         <v>98</v>

</xml_diff>